<commit_message>
added submission files to github as backup
</commit_message>
<xml_diff>
--- a/SMAA8411 A1 Submission - ST10055763 (K Maharajh).xlsx
+++ b/SMAA8411 A1 Submission - ST10055763 (K Maharajh).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiash\OneDrive\Documents\SMAA8411 Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2971697B-CF64-4249-A5FC-417E800666E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CE459E-48FD-45D2-A198-17E3265553AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{3749FFDF-EFC8-4D51-A944-337CED600082}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{3749FFDF-EFC8-4D51-A944-337CED600082}"/>
   </bookViews>
   <sheets>
     <sheet name="Q2" sheetId="2" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="312">
   <si>
     <t>stand</t>
   </si>
@@ -1035,9 +1035,6 @@
     <t>Q.3.3)</t>
   </si>
   <si>
-    <t xml:space="preserve">Git Link for my python code (referenced): </t>
-  </si>
-  <si>
     <t>If zero is within the confidence interval, then X₉ is not significant at the 5% level.</t>
   </si>
   <si>
@@ -1325,6 +1322,12 @@
   <si>
     <t>Using the mean and new vector, the following distances can be calculated:</t>
   </si>
+  <si>
+    <t>Git Link for my python code (referenced):</t>
+  </si>
+  <si>
+    <t>https://github.com/ST10055763/ST10055763-SMAA8411-A1.git</t>
+  </si>
 </sst>
 </file>
 
@@ -1495,7 +1498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1533,7 +1536,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -2406,7 +2408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9D9A5C-8790-4E73-9FF2-C6A20F140F8A}">
   <dimension ref="A1:K184"/>
   <sheetViews>
-    <sheetView zoomScale="95" workbookViewId="0">
+    <sheetView topLeftCell="A91" zoomScale="95" workbookViewId="0">
       <selection activeCell="A153" sqref="A153"/>
     </sheetView>
   </sheetViews>
@@ -5222,10 +5224,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85DF63D0-2F1F-47D9-A38E-20DAA1472685}">
-  <dimension ref="A1:U468"/>
+  <dimension ref="A1:Z468"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScale="93" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q79" sqref="Q79"/>
+    <sheetView tabSelected="1" topLeftCell="J64" zoomScale="93" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U78" sqref="U78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8786,7 +8788,7 @@
         <v>-8.2072681987270341E-11</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>45</v>
       </c>
@@ -8843,7 +8845,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>35</v>
       </c>
@@ -8894,7 +8896,7 @@
         <v>-3.3348972763923781E-5</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>0</v>
       </c>
@@ -8951,7 +8953,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>0</v>
       </c>
@@ -9002,7 +9004,7 @@
         <v>-0.11799250833649502</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>0</v>
       </c>
@@ -9056,7 +9058,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>0</v>
       </c>
@@ -9114,7 +9116,7 @@
         <v>6.900202887987425E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>0</v>
       </c>
@@ -9171,7 +9173,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>0</v>
       </c>
@@ -9222,7 +9224,7 @@
         <v>-6.069492593619656E-9</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>0</v>
       </c>
@@ -9275,11 +9277,16 @@
       <c r="R73" t="s">
         <v>278</v>
       </c>
-      <c r="U73" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U73" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="V73" s="25"/>
+      <c r="W73" s="25"/>
+      <c r="X73" s="25"/>
+      <c r="Y73" s="25"/>
+      <c r="Z73" s="25"/>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>0</v>
       </c>
@@ -9329,8 +9336,16 @@
         <f>LN(Table5[[#This Row],[probability]])</f>
         <v>-0.2902022480532559</v>
       </c>
-    </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U74" s="25" t="s">
+        <v>311</v>
+      </c>
+      <c r="V74" s="25"/>
+      <c r="W74" s="25"/>
+      <c r="X74" s="25"/>
+      <c r="Y74" s="25"/>
+      <c r="Z74" s="25"/>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>0</v>
       </c>
@@ -9384,7 +9399,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>0</v>
       </c>
@@ -9438,7 +9453,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>0</v>
       </c>
@@ -9492,7 +9507,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>0</v>
       </c>
@@ -9543,7 +9558,7 @@
         <v>-1.045622590632029E-5</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>0</v>
       </c>
@@ -9597,10 +9612,10 @@
         <v>282</v>
       </c>
       <c r="R79" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>0</v>
       </c>
@@ -9651,7 +9666,7 @@
         <v>-9.4727220715017477E-2</v>
       </c>
       <c r="R80" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.3">
@@ -9705,7 +9720,7 @@
         <v>-0.18067414502312598</v>
       </c>
       <c r="R81" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.3">
@@ -9810,7 +9825,7 @@
         <v>-1.8145031429819932E-5</v>
       </c>
       <c r="R83" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.3">
@@ -9864,7 +9879,7 @@
         <v>-5.5564201229466064E-8</v>
       </c>
       <c r="R84" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.3">
@@ -9969,7 +9984,7 @@
         <v>-0.20774523585814456</v>
       </c>
       <c r="R86" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.3">
@@ -30255,8 +30270,8 @@
       <c r="G38" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="H38" s="25" t="s">
-        <v>299</v>
+      <c r="H38" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
@@ -30275,8 +30290,8 @@
       <c r="E39" t="s">
         <v>233</v>
       </c>
-      <c r="H39" s="25" t="s">
-        <v>300</v>
+      <c r="H39" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
@@ -30313,10 +30328,10 @@
         <v>233</v>
       </c>
       <c r="H41" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M41" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
@@ -30436,8 +30451,8 @@
       <c r="E46" t="s">
         <v>233</v>
       </c>
-      <c r="H46" s="25" t="s">
-        <v>302</v>
+      <c r="H46" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
@@ -30508,7 +30523,7 @@
         <v>233</v>
       </c>
       <c r="H50" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -30528,7 +30543,7 @@
         <v>233</v>
       </c>
       <c r="H51" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I51">
         <f>SQRT((N42 - I12)^2 + (N43 - I13)^2 + (N44 - I14)^2 + (N45 - I15)^2)</f>
@@ -30551,10 +30566,10 @@
       <c r="E52" t="s">
         <v>234</v>
       </c>
-      <c r="H52" s="26" t="s">
-        <v>304</v>
-      </c>
-      <c r="I52" s="26">
+      <c r="H52" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="I52" s="25">
         <f>SQRT((N42 - I19)^2 + (N43 - I20)^2 + (N44 - I21)^2 + (N45 - I22)^2)</f>
         <v>1.0850216587699986</v>
       </c>
@@ -30576,7 +30591,7 @@
         <v>234</v>
       </c>
       <c r="H53" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I53">
         <f>SQRT((N42 - I26)^2 + (N43 - I27)^2 + (N44 - I28)^2 + (N45 - I29)^2)</f>
@@ -30617,7 +30632,7 @@
         <v>234</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -30636,8 +30651,8 @@
       <c r="E56" t="s">
         <v>234</v>
       </c>
-      <c r="H56" s="25" t="s">
-        <v>308</v>
+      <c r="H56" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
@@ -32274,7 +32289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2BADF5-C35F-4B99-B896-E3602C8BDE5F}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
@@ -32282,52 +32297,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>